<commit_message>
succese item task file name 50.0062 and file name 50.0063
</commit_message>
<xml_diff>
--- a/Arif0624/Arif0624.xlsx
+++ b/Arif0624/Arif0624.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Scraping\Don Osterloh\Scraping data\Arif0624\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F5390C-4313-47C1-B113-11BB8AA5F95B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF56F88-3278-4A3A-BA3E-1E26FF3FE6BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{2528E7F7-C8C7-944B-ACBE-D4E95E4C88D2}"/>
   </bookViews>
@@ -193,9 +193,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="12">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -227,8 +234,48 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Eurostile"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Eurostile"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -244,6 +291,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -274,30 +333,79 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -615,8 +723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7221CAC1-3680-1942-A1A6-CE5928425F1C}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView showFormulas="1" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -626,353 +734,353 @@
     <col min="4" max="4" width="51.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:8" s="9" customFormat="1" ht="28.5" customHeight="1">
+      <c r="A1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H1" s="4"/>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="1">
+      <c r="H1" s="8"/>
+    </row>
+    <row r="2" spans="1:8" s="9" customFormat="1" ht="28.5" customHeight="1">
+      <c r="A2" s="10">
         <v>50.041800000000002</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="4"/>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="1">
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="8"/>
+    </row>
+    <row r="3" spans="1:8" s="9" customFormat="1" ht="28.5" customHeight="1">
+      <c r="A3" s="10">
         <v>50.041899999999998</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="4"/>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="1">
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="8"/>
+    </row>
+    <row r="4" spans="1:8" s="9" customFormat="1" ht="28.5" customHeight="1">
+      <c r="A4" s="10">
         <v>50.042000000000002</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="4"/>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="1">
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="8"/>
+    </row>
+    <row r="5" spans="1:8" s="18" customFormat="1" ht="28.5" customHeight="1">
+      <c r="A5" s="14">
         <v>40.1145</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="4"/>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="1">
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="17"/>
+    </row>
+    <row r="6" spans="1:8" s="9" customFormat="1" ht="28.5" customHeight="1">
+      <c r="A6" s="10">
         <v>40.114699999999999</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="4"/>
-    </row>
-    <row r="7" spans="1:8" s="12" customFormat="1">
-      <c r="A7" s="8">
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="8"/>
+    </row>
+    <row r="7" spans="1:8" s="23" customFormat="1" ht="28.5" customHeight="1">
+      <c r="A7" s="19">
         <v>50.041499999999999</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="11"/>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="1">
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="22"/>
+    </row>
+    <row r="8" spans="1:8" s="9" customFormat="1" ht="28.5" customHeight="1">
+      <c r="A8" s="10">
         <v>50.041600000000003</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="4"/>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="1">
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="8"/>
+    </row>
+    <row r="9" spans="1:8" s="9" customFormat="1" ht="28.5" customHeight="1">
+      <c r="A9" s="10">
         <v>50.041699999999999</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="4"/>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="1">
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="8"/>
+    </row>
+    <row r="10" spans="1:8" s="9" customFormat="1" ht="28.5" customHeight="1">
+      <c r="A10" s="10">
         <v>60.009</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="4"/>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="1">
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="8"/>
+    </row>
+    <row r="11" spans="1:8" s="9" customFormat="1" ht="28.5" customHeight="1">
+      <c r="A11" s="10">
         <v>50.005699999999997</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="4"/>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="1">
+      <c r="G11" s="11"/>
+      <c r="H11" s="8"/>
+    </row>
+    <row r="12" spans="1:8" s="9" customFormat="1" ht="28.5" customHeight="1">
+      <c r="A12" s="10">
         <v>50.005800000000001</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="G12" s="2"/>
-      <c r="H12" s="4"/>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="1">
+      <c r="G12" s="11"/>
+      <c r="H12" s="8"/>
+    </row>
+    <row r="13" spans="1:8" s="9" customFormat="1" ht="28.5" customHeight="1">
+      <c r="A13" s="10">
         <v>50.005899999999997</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="G13" s="2"/>
-      <c r="H13" s="4"/>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="1">
+      <c r="G13" s="11"/>
+      <c r="H13" s="8"/>
+    </row>
+    <row r="14" spans="1:8" s="9" customFormat="1" ht="28.5" customHeight="1">
+      <c r="A14" s="10">
         <v>50.006</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="G14" s="2"/>
-      <c r="H14" s="4"/>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="1">
+      <c r="G14" s="11"/>
+      <c r="H14" s="8"/>
+    </row>
+    <row r="15" spans="1:8" s="9" customFormat="1" ht="28.5" customHeight="1">
+      <c r="A15" s="10">
         <v>50.006100000000004</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G15" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="H15" s="4"/>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="1">
+      <c r="H15" s="8"/>
+    </row>
+    <row r="16" spans="1:8" s="7" customFormat="1" ht="28.5" customHeight="1">
+      <c r="A16" s="3">
         <v>50.0062</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G16" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="H16" s="4"/>
-    </row>
-    <row r="17" spans="1:8" s="12" customFormat="1">
-      <c r="A17" s="8">
+      <c r="H16" s="6"/>
+    </row>
+    <row r="17" spans="1:8" s="7" customFormat="1" ht="28.5" customHeight="1">
+      <c r="A17" s="3">
         <v>50.006300000000003</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="E17" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F17" s="9" t="s">
+      <c r="F17" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="G17" s="9" t="s">
+      <c r="G17" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="H17" s="11"/>
+      <c r="H17" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -985,6 +1093,8 @@
     <hyperlink ref="C10" r:id="rId7" xr:uid="{9367BCDC-06EC-4F94-8D00-B28168B6F5D8}"/>
     <hyperlink ref="C17" r:id="rId8" display="https://journaldemonaco.gouv.mc/content/search?SearchText=&amp;filter[]=attr_theme_s:%22Licenciements%22&amp;activeFacets[attr_theme_s:Th%C3%A8mes]=Licenciements&amp;activeFacets[article_jdm/category:Cat%C3%A9gories]=Avis%20et%20Communiqu%C3%A9s&amp;sort=published_desc&amp;page_limit=15" xr:uid="{1BBCFC78-98FD-4796-8666-36D1FC777A0A}"/>
     <hyperlink ref="C16" r:id="rId9" display="https://journaldemonaco.gouv.mc/content/search?SearchText=&amp;filter[]=attr_theme_s:%22R%C3%A9vocation%22&amp;activeFacets[attr_theme_s:Th%C3%A8mes]=R%C3%A9vocation&amp;activeFacets[article_jdm/category:Cat%C3%A9gories]=Avis%20et%20Communiqu%C3%A9s&amp;sort=published_desc&amp;page_limit=15" xr:uid="{097CAC81-485A-4E9D-A58F-739A8A35FDF3}"/>
+    <hyperlink ref="C6" r:id="rId10" xr:uid="{3CC76CB7-4C92-41C3-B737-EF4C93C45B98}"/>
+    <hyperlink ref="C11" r:id="rId11" xr:uid="{38A3122C-2164-4343-9809-62C38C2A82D2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
succes task 50.0417 / 50.0416 / 50.0415
</commit_message>
<xml_diff>
--- a/Arif0624/Arif0624.xlsx
+++ b/Arif0624/Arif0624.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Scraping\Don Osterloh\Scraping data\Arif0624\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Scraping\Don Osterloh\Scraping data\Arif0624\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF56F88-3278-4A3A-BA3E-1E26FF3FE6BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EAAE907-62CB-4528-86E0-6397B78B5562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{2528E7F7-C8C7-944B-ACBE-D4E95E4C88D2}"/>
   </bookViews>
@@ -129,9 +129,6 @@
     <t>Court of Appeal Case Law</t>
   </si>
   <si>
-    <t>https://www.legimonaco.mc/305//legismc.nsf/ViewJurisCA!OpenView</t>
-  </si>
-  <si>
     <t>Court of Review</t>
   </si>
   <si>
@@ -187,13 +184,16 @@
   </si>
   <si>
     <t>Notes3</t>
+  </si>
+  <si>
+    <t>https://www.legimonaco.mc/305/legismc.nsf/ViewJurisCA!OpenView</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -274,8 +274,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Eurostile"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -303,6 +309,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -335,7 +353,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -376,6 +394,75 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -386,24 +473,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -723,8 +792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7221CAC1-3680-1942-A1A6-CE5928425F1C}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView showFormulas="1" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView showFormulas="1" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -736,25 +805,25 @@
   <sheetData>
     <row r="1" spans="1:8" s="9" customFormat="1" ht="28.5" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="H1" s="8"/>
     </row>
@@ -814,23 +883,23 @@
       <c r="G4" s="11"/>
       <c r="H4" s="8"/>
     </row>
-    <row r="5" spans="1:8" s="18" customFormat="1" ht="28.5" customHeight="1">
-      <c r="A5" s="14">
+    <row r="5" spans="1:8" s="15" customFormat="1" ht="28.5" customHeight="1">
+      <c r="A5" s="33">
         <v>40.1145</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="17"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="36"/>
     </row>
     <row r="6" spans="1:8" s="9" customFormat="1" ht="28.5" customHeight="1">
       <c r="A6" s="10">
@@ -850,59 +919,59 @@
       <c r="G6" s="11"/>
       <c r="H6" s="8"/>
     </row>
-    <row r="7" spans="1:8" s="23" customFormat="1" ht="28.5" customHeight="1">
-      <c r="A7" s="19">
+    <row r="7" spans="1:8" s="14" customFormat="1" ht="28.5" customHeight="1">
+      <c r="A7" s="24">
         <v>50.041499999999999</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="22"/>
-    </row>
-    <row r="8" spans="1:8" s="9" customFormat="1" ht="28.5" customHeight="1">
-      <c r="A8" s="10">
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="27"/>
+    </row>
+    <row r="8" spans="1:8" s="14" customFormat="1" ht="28.5" customHeight="1">
+      <c r="A8" s="37">
         <v>50.041600000000003</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="8"/>
-    </row>
-    <row r="9" spans="1:8" s="9" customFormat="1" ht="28.5" customHeight="1">
-      <c r="A9" s="10">
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="40"/>
+    </row>
+    <row r="9" spans="1:8" s="14" customFormat="1" ht="28.5" customHeight="1">
+      <c r="A9" s="37">
         <v>50.041699999999999</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="8"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="40"/>
     </row>
     <row r="10" spans="1:8" s="9" customFormat="1" ht="28.5" customHeight="1">
       <c r="A10" s="10">
@@ -922,139 +991,139 @@
       <c r="G10" s="11"/>
       <c r="H10" s="8"/>
     </row>
-    <row r="11" spans="1:8" s="9" customFormat="1" ht="28.5" customHeight="1">
-      <c r="A11" s="10">
+    <row r="11" spans="1:8" s="22" customFormat="1" ht="28.5" customHeight="1">
+      <c r="A11" s="19">
         <v>50.005699999999997</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F11" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="G11" s="11"/>
-      <c r="H11" s="8"/>
-    </row>
-    <row r="12" spans="1:8" s="9" customFormat="1" ht="28.5" customHeight="1">
-      <c r="A12" s="10">
+      <c r="G11" s="20"/>
+      <c r="H11" s="21"/>
+    </row>
+    <row r="12" spans="1:8" s="22" customFormat="1" ht="28.5" customHeight="1">
+      <c r="A12" s="19">
         <v>50.005800000000001</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="20"/>
+      <c r="H12" s="21"/>
+    </row>
+    <row r="13" spans="1:8" s="22" customFormat="1" ht="28.5" customHeight="1">
+      <c r="A13" s="19">
+        <v>50.005899999999997</v>
+      </c>
+      <c r="B13" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="C13" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E13" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="F12" s="11" t="s">
+      <c r="F13" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="G12" s="11"/>
-      <c r="H12" s="8"/>
-    </row>
-    <row r="13" spans="1:8" s="9" customFormat="1" ht="28.5" customHeight="1">
-      <c r="A13" s="10">
-        <v>50.005899999999997</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="13" t="s">
+      <c r="G13" s="20"/>
+      <c r="H13" s="21"/>
+    </row>
+    <row r="14" spans="1:8" s="22" customFormat="1" ht="28.5" customHeight="1">
+      <c r="A14" s="19">
+        <v>50.006</v>
+      </c>
+      <c r="B14" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="C14" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E14" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="F14" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="G13" s="11"/>
-      <c r="H13" s="8"/>
-    </row>
-    <row r="14" spans="1:8" s="9" customFormat="1" ht="28.5" customHeight="1">
-      <c r="A14" s="10">
-        <v>50.006</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" s="13" t="s">
+      <c r="G14" s="20"/>
+      <c r="H14" s="21"/>
+    </row>
+    <row r="15" spans="1:8" s="32" customFormat="1" ht="28.5" customHeight="1">
+      <c r="A15" s="28">
+        <v>50.006100000000004</v>
+      </c>
+      <c r="B15" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="G14" s="11"/>
-      <c r="H14" s="8"/>
-    </row>
-    <row r="15" spans="1:8" s="9" customFormat="1" ht="28.5" customHeight="1">
-      <c r="A15" s="10">
-        <v>50.006100000000004</v>
-      </c>
-      <c r="B15" s="11" t="s">
+      <c r="C15" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="D15" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="E15" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="E15" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="G15" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="H15" s="8"/>
+      <c r="F15" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="G15" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="H15" s="31"/>
     </row>
     <row r="16" spans="1:8" s="7" customFormat="1" ht="28.5" customHeight="1">
       <c r="A16" s="3">
         <v>50.0062</v>
       </c>
       <c r="B16" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>41</v>
-      </c>
       <c r="D16" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E16" s="4" t="s">
-        <v>39</v>
-      </c>
       <c r="F16" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H16" s="6"/>
     </row>
@@ -1063,22 +1132,22 @@
         <v>50.006300000000003</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>43</v>
-      </c>
       <c r="D17" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E17" s="4" t="s">
-        <v>39</v>
-      </c>
       <c r="F17" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H17" s="6"/>
     </row>
@@ -1095,6 +1164,9 @@
     <hyperlink ref="C16" r:id="rId9" display="https://journaldemonaco.gouv.mc/content/search?SearchText=&amp;filter[]=attr_theme_s:%22R%C3%A9vocation%22&amp;activeFacets[attr_theme_s:Th%C3%A8mes]=R%C3%A9vocation&amp;activeFacets[article_jdm/category:Cat%C3%A9gories]=Avis%20et%20Communiqu%C3%A9s&amp;sort=published_desc&amp;page_limit=15" xr:uid="{097CAC81-485A-4E9D-A58F-739A8A35FDF3}"/>
     <hyperlink ref="C6" r:id="rId10" xr:uid="{3CC76CB7-4C92-41C3-B737-EF4C93C45B98}"/>
     <hyperlink ref="C11" r:id="rId11" xr:uid="{38A3122C-2164-4343-9809-62C38C2A82D2}"/>
+    <hyperlink ref="C12" r:id="rId12" xr:uid="{5A968074-F77A-4827-8057-F67C97DB7FBD}"/>
+    <hyperlink ref="C15" r:id="rId13" display="https://journaldemonaco.gouv.mc/content/search?SearchText=&amp;filter[]=attr_theme_s:%22Extraits%20Judiciaires%22&amp;activeFacets[attr_theme_s:Th%C3%A8mes]=Extraits%20Judiciaires&amp;activeFacets[attr_category_s:Cat%C3%A9gories]=Insertions%20l%C3%A9gales%20et%20Annonces&amp;activeFacets[article_jdm/category:Cat%C3%A9gories]=Insertions%20l%C3%A9gales%20et%20Annonces&amp;filter[]=attr_category_s:%22Insertions%20l%C3%A9gales%20et%20Annonces%22&amp;sort=published_desc&amp;page_limit=15" xr:uid="{5AD4AA26-1F8B-45E2-8EAE-586129424765}"/>
+    <hyperlink ref="C14" r:id="rId14" xr:uid="{680DEF4A-FF34-485E-9061-62700B880648}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
succes add page pagination task 40.1145
</commit_message>
<xml_diff>
--- a/Arif0624/Arif0624.xlsx
+++ b/Arif0624/Arif0624.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Scraping\Don Osterloh\Scraping data\Arif0624\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EAAE907-62CB-4528-86E0-6397B78B5562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A2FEBF1-D61C-441E-AEAA-E3C0FEC15045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{2528E7F7-C8C7-944B-ACBE-D4E95E4C88D2}"/>
   </bookViews>
@@ -193,7 +193,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -211,12 +211,6 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Eurostile"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color rgb="FF0563C1"/>
       <name val="Eurostile"/>
     </font>
     <font>
@@ -281,7 +275,7 @@
       <name val="Eurostile"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -308,19 +302,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -351,9 +333,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -361,22 +343,22 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -388,79 +370,43 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -469,10 +415,10 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -792,8 +738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7221CAC1-3680-1942-A1A6-CE5928425F1C}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView showFormulas="1" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView showFormulas="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -852,7 +798,7 @@
       <c r="B3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="12" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="11" t="s">
@@ -883,23 +829,23 @@
       <c r="G4" s="11"/>
       <c r="H4" s="8"/>
     </row>
-    <row r="5" spans="1:8" s="15" customFormat="1" ht="28.5" customHeight="1">
-      <c r="A5" s="33">
+    <row r="5" spans="1:8" s="13" customFormat="1" ht="28.5" customHeight="1">
+      <c r="A5" s="25">
         <v>40.1145</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="34" t="s">
+      <c r="D5" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="36"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="28"/>
     </row>
     <row r="6" spans="1:8" s="9" customFormat="1" ht="28.5" customHeight="1">
       <c r="A6" s="10">
@@ -919,189 +865,189 @@
       <c r="G6" s="11"/>
       <c r="H6" s="8"/>
     </row>
-    <row r="7" spans="1:8" s="14" customFormat="1" ht="28.5" customHeight="1">
-      <c r="A7" s="24">
+    <row r="7" spans="1:8" s="13" customFormat="1" ht="28.5" customHeight="1">
+      <c r="A7" s="21">
         <v>50.041499999999999</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="27"/>
-    </row>
-    <row r="8" spans="1:8" s="14" customFormat="1" ht="28.5" customHeight="1">
-      <c r="A8" s="37">
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="24"/>
+    </row>
+    <row r="8" spans="1:8" s="13" customFormat="1" ht="28.5" customHeight="1">
+      <c r="A8" s="25">
         <v>50.041600000000003</v>
       </c>
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="39" t="s">
+      <c r="C8" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="38" t="s">
+      <c r="D8" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="40"/>
-    </row>
-    <row r="9" spans="1:8" s="14" customFormat="1" ht="28.5" customHeight="1">
-      <c r="A9" s="37">
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="28"/>
+    </row>
+    <row r="9" spans="1:8" s="7" customFormat="1" ht="28.5" customHeight="1">
+      <c r="A9" s="3">
         <v>50.041699999999999</v>
       </c>
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="39" t="s">
+      <c r="C9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="38" t="s">
+      <c r="D9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="40"/>
-    </row>
-    <row r="10" spans="1:8" s="9" customFormat="1" ht="28.5" customHeight="1">
-      <c r="A10" s="10">
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="6"/>
+    </row>
+    <row r="10" spans="1:8" s="7" customFormat="1" ht="28.5" customHeight="1">
+      <c r="A10" s="3">
         <v>60.009</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="8"/>
-    </row>
-    <row r="11" spans="1:8" s="22" customFormat="1" ht="28.5" customHeight="1">
-      <c r="A11" s="19">
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="6"/>
+    </row>
+    <row r="11" spans="1:8" s="19" customFormat="1" ht="28.5" customHeight="1">
+      <c r="A11" s="16">
         <v>50.005699999999997</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="20" t="s">
+      <c r="E11" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="20" t="s">
+      <c r="F11" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="G11" s="20"/>
-      <c r="H11" s="21"/>
-    </row>
-    <row r="12" spans="1:8" s="22" customFormat="1" ht="28.5" customHeight="1">
-      <c r="A12" s="19">
+      <c r="G11" s="17"/>
+      <c r="H11" s="18"/>
+    </row>
+    <row r="12" spans="1:8" s="19" customFormat="1" ht="28.5" customHeight="1">
+      <c r="A12" s="16">
         <v>50.005800000000001</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="20" t="s">
+      <c r="D12" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="20" t="s">
+      <c r="E12" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="F12" s="20" t="s">
+      <c r="F12" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="G12" s="20"/>
-      <c r="H12" s="21"/>
-    </row>
-    <row r="13" spans="1:8" s="22" customFormat="1" ht="28.5" customHeight="1">
-      <c r="A13" s="19">
+      <c r="G12" s="17"/>
+      <c r="H12" s="18"/>
+    </row>
+    <row r="13" spans="1:8" s="19" customFormat="1" ht="28.5" customHeight="1">
+      <c r="A13" s="16">
         <v>50.005899999999997</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="20" t="s">
+      <c r="D13" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="20" t="s">
+      <c r="E13" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="F13" s="20" t="s">
+      <c r="F13" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="G13" s="20"/>
-      <c r="H13" s="21"/>
-    </row>
-    <row r="14" spans="1:8" s="22" customFormat="1" ht="28.5" customHeight="1">
-      <c r="A14" s="19">
+      <c r="G13" s="17"/>
+      <c r="H13" s="18"/>
+    </row>
+    <row r="14" spans="1:8" s="19" customFormat="1" ht="28.5" customHeight="1">
+      <c r="A14" s="16">
         <v>50.006</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="20" t="s">
+      <c r="D14" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="20" t="s">
+      <c r="E14" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="F14" s="20" t="s">
+      <c r="F14" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="G14" s="20"/>
-      <c r="H14" s="21"/>
-    </row>
-    <row r="15" spans="1:8" s="32" customFormat="1" ht="28.5" customHeight="1">
-      <c r="A15" s="28">
+      <c r="G14" s="17"/>
+      <c r="H14" s="18"/>
+    </row>
+    <row r="15" spans="1:8" s="7" customFormat="1" ht="28.5" customHeight="1">
+      <c r="A15" s="3">
         <v>50.006100000000004</v>
       </c>
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="30" t="s">
+      <c r="C15" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="29" t="s">
+      <c r="D15" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E15" s="29" t="s">
+      <c r="E15" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F15" s="29" t="s">
+      <c r="F15" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="G15" s="29" t="s">
+      <c r="G15" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="H15" s="31"/>
+      <c r="H15" s="6"/>
     </row>
     <row r="16" spans="1:8" s="7" customFormat="1" ht="28.5" customHeight="1">
       <c r="A16" s="3">
@@ -1134,7 +1080,7 @@
       <c r="B17" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="5" t="s">
         <v>42</v>
       </c>
       <c r="D17" s="4" t="s">
@@ -1167,7 +1113,9 @@
     <hyperlink ref="C12" r:id="rId12" xr:uid="{5A968074-F77A-4827-8057-F67C97DB7FBD}"/>
     <hyperlink ref="C15" r:id="rId13" display="https://journaldemonaco.gouv.mc/content/search?SearchText=&amp;filter[]=attr_theme_s:%22Extraits%20Judiciaires%22&amp;activeFacets[attr_theme_s:Th%C3%A8mes]=Extraits%20Judiciaires&amp;activeFacets[attr_category_s:Cat%C3%A9gories]=Insertions%20l%C3%A9gales%20et%20Annonces&amp;activeFacets[article_jdm/category:Cat%C3%A9gories]=Insertions%20l%C3%A9gales%20et%20Annonces&amp;filter[]=attr_category_s:%22Insertions%20l%C3%A9gales%20et%20Annonces%22&amp;sort=published_desc&amp;page_limit=15" xr:uid="{5AD4AA26-1F8B-45E2-8EAE-586129424765}"/>
     <hyperlink ref="C14" r:id="rId14" xr:uid="{680DEF4A-FF34-485E-9061-62700B880648}"/>
+    <hyperlink ref="C3" r:id="rId15" xr:uid="{0CA96EC9-603F-4BB6-8A51-F2B2FF7C7B13}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>